<commit_message>
RLS include Manager Role to view all
</commit_message>
<xml_diff>
--- a/RLS.xlsx
+++ b/RLS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://majescogroup-my.sharepoint.com/personal/david910219_majesco_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workarea\sample\Embed-API-Sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{5C83A7F6-2E95-4C5C-A593-5401578D9F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B55D36D6-B19A-402E-B6D7-A2A5AD9FC5B5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223BD52-C2E6-47D8-890C-3942E7FA7E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="4170" windowWidth="21600" windowHeight="11295" xr2:uid="{05B2E61A-63F8-42AC-92AB-A4F7902674B0}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{05B2E61A-63F8-42AC-92AB-A4F7902674B0}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>UserID</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Project 6</t>
+  </si>
+  <si>
+    <t>user1@majesco.com</t>
+  </si>
+  <si>
+    <t>user2@majesco.com</t>
+  </si>
+  <si>
+    <t>user3@majesco.com</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
@@ -139,10 +151,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,48 +470,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DB7C5D-5124-4612-977B-285962CE82AD}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -511,6 +564,10 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{CB4FA995-1509-426E-B01B-6664119B9B9D}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{CF2BD077-F71D-40E2-A1C7-8B410034DE05}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{8A11B933-8552-416D-8E37-648AAEB565F7}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{026910BD-9358-48AF-93D9-9031CAF0E4D3}"/>
+    <hyperlink ref="B6:B7" r:id="rId5" display="user1@majesco.com" xr:uid="{C5B986B0-83F2-4882-BFC1-D7D7DB68A0C0}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{698FBECD-D6E7-4C41-9680-5B0D8D356568}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{09FB0DA9-4E42-4599-B136-CF5521822B60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -521,16 +578,16 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -552,7 +609,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -563,7 +620,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -574,7 +631,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -585,7 +642,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -596,7 +653,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>

</xml_diff>